<commit_message>
add play voice function
</commit_message>
<xml_diff>
--- a/Excels/产品功能列表20180503.xlsx
+++ b/Excels/产品功能列表20180503.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10695" windowHeight="9930" tabRatio="361"/>
+    <workbookView windowWidth="21495" windowHeight="10350" tabRatio="361"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1491,7 +1491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586">
   <si>
     <t>Medeli英文</t>
   </si>
@@ -2394,6 +2394,9 @@
     <t>Melody</t>
   </si>
   <si>
+    <t>melody</t>
+  </si>
+  <si>
     <t>旋律</t>
   </si>
   <si>
@@ -2412,12 +2415,18 @@
     <t xml:space="preserve">Metronome </t>
   </si>
   <si>
+    <t xml:space="preserve">metronome </t>
+  </si>
+  <si>
     <t>节拍器</t>
   </si>
   <si>
     <t>Microphone</t>
   </si>
   <si>
+    <t>microphone</t>
+  </si>
+  <si>
     <t>麦克风</t>
   </si>
   <si>
@@ -2448,6 +2457,9 @@
     <t>Mixer</t>
   </si>
   <si>
+    <t>mixer</t>
+  </si>
+  <si>
     <t>调音台</t>
   </si>
   <si>
@@ -2457,12 +2469,18 @@
     <t>Modulation</t>
   </si>
   <si>
+    <t>modulation</t>
+  </si>
+  <si>
     <t>颤音</t>
   </si>
   <si>
     <t>Mono</t>
   </si>
   <si>
+    <t>mono</t>
+  </si>
+  <si>
     <t>单音</t>
   </si>
   <si>
@@ -2490,6 +2508,9 @@
     <t>Octave</t>
   </si>
   <si>
+    <t>octave</t>
+  </si>
+  <si>
     <t>八度</t>
   </si>
   <si>
@@ -2502,6 +2523,9 @@
     <t>Overdrive</t>
   </si>
   <si>
+    <t>overdrive</t>
+  </si>
+  <si>
     <t>过载效果</t>
   </si>
   <si>
@@ -2541,6 +2565,9 @@
     <t>Pan</t>
   </si>
   <si>
+    <t>pan</t>
+  </si>
+  <si>
     <t>声像</t>
   </si>
   <si>
@@ -2562,6 +2589,9 @@
     <t>Pattern</t>
   </si>
   <si>
+    <t>pattern</t>
+  </si>
+  <si>
     <t>模板</t>
   </si>
   <si>
@@ -2574,6 +2604,9 @@
     <t>Pedal</t>
   </si>
   <si>
+    <t>pedal</t>
+  </si>
+  <si>
     <t>踏板</t>
   </si>
   <si>
@@ -2583,16 +2616,25 @@
     <t>Performance Assistant (Perform.)</t>
   </si>
   <si>
+    <t>performance</t>
+  </si>
+  <si>
     <t>演奏帮助</t>
   </si>
   <si>
     <t>Perform.H.</t>
   </si>
   <si>
+    <t>perform</t>
+  </si>
+  <si>
     <t>演奏帮助.高</t>
   </si>
   <si>
     <t>Polyphony（Max.)</t>
+  </si>
+  <si>
+    <t>polyphony</t>
   </si>
   <si>
     <t>复音数（最大）</t>
@@ -2678,6 +2720,9 @@
     <t>Phrase</t>
   </si>
   <si>
+    <t>phrase</t>
+  </si>
+  <si>
     <t>乐句</t>
   </si>
   <si>
@@ -2690,12 +2735,18 @@
     <t>Pilot Production (PP)</t>
   </si>
   <si>
+    <t>pilot</t>
+  </si>
+  <si>
     <t>试产</t>
   </si>
   <si>
     <t>Pitch</t>
   </si>
   <si>
+    <t>pitch</t>
+  </si>
+  <si>
     <t>音高</t>
   </si>
   <si>
@@ -2717,12 +2768,18 @@
     <t>Polarity</t>
   </si>
   <si>
+    <t>polarity</t>
+  </si>
+  <si>
     <t>极性</t>
   </si>
   <si>
     <t>Portamento</t>
   </si>
   <si>
+    <t>portamento</t>
+  </si>
+  <si>
     <t>滑音（效果）</t>
   </si>
   <si>
@@ -2759,6 +2816,9 @@
     <t>Prototype</t>
   </si>
   <si>
+    <t>prototype</t>
+  </si>
+  <si>
     <t>原型</t>
   </si>
   <si>
@@ -2771,6 +2831,9 @@
     <t>Registration Memory（Performance Memory)</t>
   </si>
   <si>
+    <t>registration</t>
+  </si>
+  <si>
     <t>注册记忆 (演奏记忆）</t>
   </si>
   <si>
@@ -2780,15 +2843,24 @@
     <t>Registration Sequence</t>
   </si>
   <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t>释音/音尾</t>
+  </si>
+  <si>
     <t xml:space="preserve">Release </t>
   </si>
   <si>
-    <t>释音/音尾</t>
-  </si>
-  <si>
     <t>Reverb</t>
   </si>
   <si>
+    <t>reverb</t>
+  </si>
+  <si>
     <t>混响</t>
   </si>
   <si>
@@ -2825,6 +2897,9 @@
     <t xml:space="preserve">Rhythm </t>
   </si>
   <si>
+    <t>rhythm</t>
+  </si>
+  <si>
     <t>打击乐</t>
   </si>
   <si>
@@ -2837,18 +2912,27 @@
     <t>Sampling</t>
   </si>
   <si>
+    <t>sampling</t>
+  </si>
+  <si>
     <t>采样</t>
   </si>
   <si>
     <t>Sample rate</t>
   </si>
   <si>
+    <t>sample</t>
+  </si>
+  <si>
     <t>采样率</t>
   </si>
   <si>
     <t>Scale</t>
   </si>
   <si>
+    <t>scale</t>
+  </si>
+  <si>
     <t>古典音律</t>
   </si>
   <si>
@@ -2879,18 +2963,27 @@
     <t>Score</t>
   </si>
   <si>
+    <t>score</t>
+  </si>
+  <si>
     <t>乐谱</t>
   </si>
   <si>
     <t>Scratching (scrubbing)</t>
   </si>
   <si>
+    <t>scratching</t>
+  </si>
+  <si>
     <t>（DJ）搓碟</t>
   </si>
   <si>
     <t>Section</t>
   </si>
   <si>
+    <t>section</t>
+  </si>
+  <si>
     <t>段落</t>
   </si>
   <si>
@@ -2921,6 +3014,9 @@
     <t>Sostenuto pedal</t>
   </si>
   <si>
+    <t>sostenuto</t>
+  </si>
+  <si>
     <t>后延音踏板</t>
   </si>
   <si>
@@ -2933,6 +3029,9 @@
     <t>Specifications</t>
   </si>
   <si>
+    <t>specifications</t>
+  </si>
+  <si>
     <t>规格</t>
   </si>
   <si>
@@ -2987,18 +3086,27 @@
     <t>Store</t>
   </si>
   <si>
+    <t>store</t>
+  </si>
+  <si>
     <t>存储</t>
   </si>
   <si>
     <t>Surround（rubber/foam）</t>
   </si>
   <si>
+    <t>surround</t>
+  </si>
+  <si>
     <t>喇叭边 (橡胶/泡沫）</t>
   </si>
   <si>
     <t>Sustain</t>
   </si>
   <si>
+    <t>sustain</t>
+  </si>
+  <si>
     <t>延音</t>
   </si>
   <si>
@@ -3038,12 +3146,18 @@
     <t>Tempo</t>
   </si>
   <si>
+    <t>tempo</t>
+  </si>
+  <si>
     <t>速度</t>
   </si>
   <si>
     <t>Tap (Tempo)</t>
   </si>
   <si>
+    <t>tap</t>
+  </si>
+  <si>
     <t>击拍设速</t>
   </si>
   <si>
@@ -3053,12 +3167,18 @@
     <t>Time signature</t>
   </si>
   <si>
+    <t>signature</t>
+  </si>
+  <si>
     <t>拍号</t>
   </si>
   <si>
     <t>Tone Generator</t>
   </si>
   <si>
+    <t>generator</t>
+  </si>
+  <si>
     <t>音源</t>
   </si>
   <si>
@@ -3068,6 +3188,9 @@
     <t>Touch</t>
   </si>
   <si>
+    <t>touch</t>
+  </si>
+  <si>
     <t>力度</t>
   </si>
   <si>
@@ -3095,18 +3218,27 @@
     <t>Transpose</t>
   </si>
   <si>
+    <t>transpose</t>
+  </si>
+  <si>
     <t>移调</t>
   </si>
   <si>
     <t>Tremelo</t>
   </si>
   <si>
+    <t>tremelo</t>
+  </si>
+  <si>
     <t>震音</t>
   </si>
   <si>
     <t>Tune</t>
   </si>
   <si>
+    <t>tune</t>
+  </si>
+  <si>
     <t>音调</t>
   </si>
   <si>
@@ -3125,6 +3257,9 @@
     <t>Tweeter</t>
   </si>
   <si>
+    <t>tweeter</t>
+  </si>
+  <si>
     <t>高音喇叭</t>
   </si>
   <si>
@@ -3179,6 +3314,9 @@
     <t>Vibrato</t>
   </si>
   <si>
+    <t>vibrato</t>
+  </si>
+  <si>
     <t>Voice</t>
   </si>
   <si>
@@ -3255,6 +3393,9 @@
   </si>
   <si>
     <t>Woofer</t>
+  </si>
+  <si>
+    <t>woofer</t>
   </si>
   <si>
     <t>低音喇叭</t>
@@ -3266,9 +3407,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -3325,6 +3466,35 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -3342,29 +3512,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3378,31 +3526,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3416,16 +3540,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3440,7 +3573,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -3448,7 +3589,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -3488,7 +3629,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3503,13 +3644,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3521,13 +3710,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3545,67 +3782,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3617,61 +3794,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3834,15 +3969,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3858,17 +3984,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3876,8 +3996,19 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3906,17 +4037,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3931,6 +4051,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -3939,10 +4074,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3951,133 +4086,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4184,7 +4319,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
@@ -4583,11 +4718,11 @@
   <dimension ref="A1:G223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A95" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="C224" sqref="C224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -6084,9 +6219,11 @@
         <v>269</v>
       </c>
       <c r="B98" s="12"/>
-      <c r="C98" s="34"/>
+      <c r="C98" s="34" t="s">
+        <v>270</v>
+      </c>
       <c r="D98" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E98" s="11" t="s">
         <v>269</v>
@@ -6096,12 +6233,14 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="11" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B99" s="12"/>
-      <c r="C99" s="12"/>
+      <c r="C99" s="34" t="s">
+        <v>270</v>
+      </c>
       <c r="D99" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E99" s="11"/>
       <c r="F99" s="14"/>
@@ -6109,12 +6248,14 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B100" s="12"/>
-      <c r="C100" s="12"/>
+      <c r="C100" s="34" t="s">
+        <v>270</v>
+      </c>
       <c r="D100" s="13" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E100" s="11"/>
       <c r="F100" s="14"/>
@@ -6122,29 +6263,33 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
+      <c r="C101" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="D101" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E101" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="E101" s="11" t="s">
-        <v>275</v>
-      </c>
       <c r="F101" s="14" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G101" s="15"/>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="11" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B102" s="12"/>
-      <c r="C102" s="12"/>
+      <c r="C102" s="12" t="s">
+        <v>280</v>
+      </c>
       <c r="D102" s="13" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E102" s="11"/>
       <c r="F102" s="14"/>
@@ -6152,12 +6297,12 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="11" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="13" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E103" s="11"/>
       <c r="F103" s="14"/>
@@ -6165,12 +6310,12 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="11" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B104" s="12"/>
       <c r="C104" s="12"/>
       <c r="D104" s="13" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E104" s="11"/>
       <c r="F104" s="14"/>
@@ -6178,12 +6323,12 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="11" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B105" s="12"/>
       <c r="C105" s="12"/>
       <c r="D105" s="13" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E105" s="11"/>
       <c r="F105" s="14"/>
@@ -6191,12 +6336,12 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="11" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B106" s="12"/>
       <c r="C106" s="12"/>
       <c r="D106" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E106" s="11"/>
       <c r="F106" s="14"/>
@@ -6204,59 +6349,65 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="11" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B107" s="12"/>
-      <c r="C107" s="12"/>
+      <c r="C107" s="12" t="s">
+        <v>291</v>
+      </c>
       <c r="D107" s="13" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F107" s="14"/>
       <c r="G107" s="15"/>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="11" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B108" s="12"/>
-      <c r="C108" s="12"/>
+      <c r="C108" s="12" t="s">
+        <v>295</v>
+      </c>
       <c r="D108" s="13" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="G108" s="15"/>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="11" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="B109" s="12"/>
-      <c r="C109" s="12"/>
+      <c r="C109" s="12" t="s">
+        <v>298</v>
+      </c>
       <c r="D109" s="13" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="F109" s="14"/>
       <c r="G109" s="15"/>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="11" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B110" s="12"/>
       <c r="C110" s="12"/>
       <c r="D110" s="13" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="E110" s="11"/>
       <c r="F110" s="14"/>
@@ -6264,27 +6415,27 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="11" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B111" s="12"/>
       <c r="C111" s="12"/>
       <c r="D111" s="13" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="E111" s="16" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="F111" s="14"/>
       <c r="G111" s="15"/>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="11" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="B112" s="12"/>
       <c r="C112" s="12"/>
       <c r="D112" s="13" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="E112" s="11"/>
       <c r="F112" s="14"/>
@@ -6292,29 +6443,33 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="11" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
+      <c r="C113" s="12" t="s">
+        <v>308</v>
+      </c>
       <c r="D113" s="13" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="G113" s="15"/>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="11" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="B114" s="12"/>
-      <c r="C114" s="12"/>
+      <c r="C114" s="12" t="s">
+        <v>313</v>
+      </c>
       <c r="D114" s="13" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="E114" s="11"/>
       <c r="F114" s="14"/>
@@ -6322,32 +6477,32 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="11" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="B115" s="12"/>
       <c r="C115" s="12"/>
       <c r="D115" s="13" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="E115" s="11" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="G115" s="15"/>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="11" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="B116" s="12"/>
       <c r="C116" s="12"/>
       <c r="D116" s="13" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="15"/>
@@ -6361,33 +6516,33 @@
       <c r="D117" s="13"/>
       <c r="E117" s="11"/>
       <c r="F117" s="14" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="G117" s="15"/>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="11" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B118" s="12"/>
       <c r="C118" s="12"/>
       <c r="D118" s="13" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="F118" s="14"/>
       <c r="G118" s="15"/>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="11" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="B119" s="12"/>
       <c r="C119" s="12"/>
       <c r="D119" s="13" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="E119" s="11"/>
       <c r="F119" s="14"/>
@@ -6395,27 +6550,31 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="11" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="B120" s="12"/>
-      <c r="C120" s="12"/>
+      <c r="C120" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="D120" s="13" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="F120" s="14"/>
       <c r="G120" s="15"/>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" s="11" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
+      <c r="C121" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="D121" s="13" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="E121" s="11"/>
       <c r="F121" s="14"/>
@@ -6423,27 +6582,31 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="11" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="B122" s="12"/>
-      <c r="C122" s="12"/>
+      <c r="C122" s="12" t="s">
+        <v>327</v>
+      </c>
       <c r="D122" s="13" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="E122" s="11"/>
       <c r="F122" s="14" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="G122" s="15"/>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="25" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="B123" s="26"/>
-      <c r="C123" s="26"/>
+      <c r="C123" s="26" t="s">
+        <v>335</v>
+      </c>
       <c r="D123" s="13" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="E123" s="11"/>
       <c r="F123" s="14"/>
@@ -6451,12 +6614,12 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="25" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="B124" s="26"/>
       <c r="C124" s="26"/>
       <c r="D124" s="13" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="E124" s="11"/>
       <c r="F124" s="14"/>
@@ -6464,25 +6627,29 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="11" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
+      <c r="C125" s="12" t="s">
+        <v>340</v>
+      </c>
       <c r="D125" s="13" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="E125" s="11"/>
       <c r="F125" s="14" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="G125" s="15"/>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="35" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="B126" s="36"/>
-      <c r="C126" s="36"/>
+      <c r="C126" s="12" t="s">
+        <v>340</v>
+      </c>
       <c r="D126" s="37" t="s">
         <v>139</v>
       </c>
@@ -6491,12 +6658,14 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="11" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
+      <c r="C127" s="12" t="s">
+        <v>344</v>
+      </c>
       <c r="D127" s="13" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="E127" s="11"/>
       <c r="F127" s="29"/>
@@ -6504,12 +6673,14 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="11" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="B128" s="12"/>
-      <c r="C128" s="12"/>
+      <c r="C128" s="12" t="s">
+        <v>347</v>
+      </c>
       <c r="D128" s="13" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="E128" s="11"/>
       <c r="F128" s="29"/>
@@ -6517,42 +6688,44 @@
     </row>
     <row r="129" ht="27" spans="1:7">
       <c r="A129" s="11" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="B129" s="12"/>
-      <c r="C129" s="12"/>
+      <c r="C129" s="12" t="s">
+        <v>350</v>
+      </c>
       <c r="D129" s="13" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="E129" s="39" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="F129" s="29"/>
       <c r="G129" s="15"/>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="19" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="B130" s="12"/>
       <c r="C130" s="12"/>
       <c r="D130" s="13" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="F130" s="29"/>
       <c r="G130" s="15"/>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="19" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="B131" s="12"/>
       <c r="C131" s="12"/>
       <c r="D131" s="13" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="E131" s="11"/>
       <c r="F131" s="29"/>
@@ -6560,12 +6733,14 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="11" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
       <c r="B132" s="12"/>
-      <c r="C132" s="12"/>
+      <c r="C132" s="12" t="s">
+        <v>359</v>
+      </c>
       <c r="D132" s="13" t="s">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="E132" s="11"/>
       <c r="F132" s="29"/>
@@ -6573,12 +6748,12 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="11" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
       <c r="B133" s="12"/>
       <c r="C133" s="12"/>
       <c r="D133" s="13" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="E133" s="11"/>
       <c r="F133" s="29"/>
@@ -6586,12 +6761,14 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="16" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
       <c r="B134" s="12"/>
-      <c r="C134" s="12"/>
+      <c r="C134" s="12" t="s">
+        <v>364</v>
+      </c>
       <c r="D134" s="13" t="s">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="E134" s="11"/>
       <c r="F134" s="29"/>
@@ -6599,12 +6776,14 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="11" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
       <c r="B135" s="12"/>
-      <c r="C135" s="12"/>
+      <c r="C135" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="D135" s="13" t="s">
-        <v>351</v>
+        <v>368</v>
       </c>
       <c r="E135" s="11"/>
       <c r="F135" s="29"/>
@@ -6612,18 +6791,20 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="11" t="s">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="B136" s="12"/>
-      <c r="C136" s="12"/>
+      <c r="C136" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="D136" s="13" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>354</v>
+        <v>371</v>
       </c>
       <c r="F136" s="14" t="s">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="G136" s="15"/>
     </row>
@@ -6632,9 +6813,11 @@
         <v>102</v>
       </c>
       <c r="B137" s="12"/>
-      <c r="C137" s="12"/>
+      <c r="C137" s="12" t="s">
+        <v>367</v>
+      </c>
       <c r="D137" s="13" t="s">
-        <v>356</v>
+        <v>373</v>
       </c>
       <c r="E137" s="11"/>
       <c r="F137" s="14"/>
@@ -6642,12 +6825,14 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138" s="16" t="s">
-        <v>357</v>
+        <v>374</v>
       </c>
       <c r="B138" s="12"/>
-      <c r="C138" s="12"/>
+      <c r="C138" s="12" t="s">
+        <v>375</v>
+      </c>
       <c r="D138" s="13" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="E138" s="11"/>
       <c r="F138" s="14"/>
@@ -6655,44 +6840,46 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139" s="16" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="B139" s="12"/>
-      <c r="C139" s="12"/>
+      <c r="C139" s="12" t="s">
+        <v>378</v>
+      </c>
       <c r="D139" s="13" t="s">
-        <v>360</v>
+        <v>379</v>
       </c>
       <c r="E139" s="11" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="F139" s="14" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="G139" s="15"/>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="11" t="s">
-        <v>361</v>
+        <v>380</v>
       </c>
       <c r="B140" s="12"/>
       <c r="C140" s="12"/>
       <c r="D140" s="13" t="s">
-        <v>362</v>
+        <v>381</v>
       </c>
       <c r="E140" s="11" t="s">
-        <v>363</v>
+        <v>382</v>
       </c>
       <c r="F140" s="14"/>
       <c r="G140" s="15"/>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" s="11" t="s">
-        <v>364</v>
+        <v>383</v>
       </c>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
       <c r="D141" s="13" t="s">
-        <v>365</v>
+        <v>384</v>
       </c>
       <c r="E141" s="11"/>
       <c r="F141" s="14"/>
@@ -6707,18 +6894,18 @@
       <c r="D142" s="13"/>
       <c r="E142" s="11"/>
       <c r="F142" s="14" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
       <c r="G142" s="15"/>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="11" t="s">
-        <v>367</v>
+        <v>386</v>
       </c>
       <c r="B143" s="12"/>
       <c r="C143" s="12"/>
       <c r="D143" s="13" t="s">
-        <v>368</v>
+        <v>387</v>
       </c>
       <c r="E143" s="11"/>
       <c r="F143" s="14"/>
@@ -6726,12 +6913,12 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="11" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
       <c r="B144" s="12"/>
       <c r="C144" s="12"/>
       <c r="D144" s="13" t="s">
-        <v>370</v>
+        <v>389</v>
       </c>
       <c r="E144" s="11"/>
       <c r="F144" s="14"/>
@@ -6739,12 +6926,14 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145" s="40" t="s">
-        <v>371</v>
+        <v>390</v>
       </c>
       <c r="B145" s="22"/>
-      <c r="C145" s="22"/>
+      <c r="C145" s="22" t="s">
+        <v>391</v>
+      </c>
       <c r="D145" s="41" t="s">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="E145" s="41"/>
       <c r="F145" s="42"/>
@@ -6752,106 +6941,118 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="11" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="B146" s="12"/>
       <c r="C146" s="12"/>
       <c r="D146" s="13" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="E146" s="11" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="F146" s="14"/>
       <c r="G146" s="15"/>
     </row>
     <row r="147" ht="27" spans="1:7">
       <c r="A147" s="43" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="B147" s="44"/>
-      <c r="C147" s="44"/>
+      <c r="C147" s="44" t="s">
+        <v>396</v>
+      </c>
       <c r="D147" s="13" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="E147" s="11" t="s">
-        <v>377</v>
+        <v>398</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>378</v>
+        <v>399</v>
       </c>
       <c r="G147" s="15"/>
     </row>
     <row r="148" spans="1:7">
       <c r="A148" s="43" t="s">
-        <v>379</v>
+        <v>400</v>
       </c>
       <c r="B148" s="44"/>
-      <c r="C148" s="44"/>
+      <c r="C148" s="44" t="s">
+        <v>401</v>
+      </c>
       <c r="D148" s="13" t="s">
-        <v>380</v>
+        <v>402</v>
       </c>
       <c r="E148" s="11" t="s">
-        <v>379</v>
+        <v>403</v>
       </c>
       <c r="F148" s="14"/>
       <c r="G148" s="15"/>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="16" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="B149" s="12"/>
-      <c r="C149" s="12"/>
+      <c r="C149" s="12" t="s">
+        <v>405</v>
+      </c>
       <c r="D149" s="13" t="s">
-        <v>382</v>
+        <v>406</v>
       </c>
       <c r="E149" s="11" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="F149" s="14" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="G149" s="15"/>
     </row>
     <row r="150" spans="1:7">
       <c r="A150" s="11" t="s">
-        <v>383</v>
+        <v>407</v>
       </c>
       <c r="B150" s="12"/>
-      <c r="C150" s="12"/>
+      <c r="C150" s="12" t="s">
+        <v>405</v>
+      </c>
       <c r="D150" s="13" t="s">
-        <v>384</v>
+        <v>408</v>
       </c>
       <c r="E150" s="11" t="s">
-        <v>385</v>
+        <v>409</v>
       </c>
       <c r="F150" s="14"/>
       <c r="G150" s="15"/>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="16" t="s">
-        <v>386</v>
+        <v>410</v>
       </c>
       <c r="B151" s="12"/>
-      <c r="C151" s="12"/>
+      <c r="C151" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="D151" s="13" t="s">
-        <v>387</v>
+        <v>411</v>
       </c>
       <c r="E151" s="11" t="s">
-        <v>386</v>
+        <v>410</v>
       </c>
       <c r="F151" s="14"/>
       <c r="G151" s="15"/>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" s="11" t="s">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="B152" s="12"/>
-      <c r="C152" s="12"/>
+      <c r="C152" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="D152" s="13" t="s">
-        <v>389</v>
+        <v>413</v>
       </c>
       <c r="E152" s="11"/>
       <c r="F152" s="14"/>
@@ -6859,57 +7060,61 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153" s="11" t="s">
-        <v>390</v>
+        <v>414</v>
       </c>
       <c r="B153" s="12"/>
       <c r="C153" s="12"/>
       <c r="D153" s="13" t="s">
-        <v>391</v>
+        <v>415</v>
       </c>
       <c r="E153" s="11"/>
       <c r="F153" s="14" t="s">
-        <v>392</v>
+        <v>416</v>
       </c>
       <c r="G153" s="15"/>
     </row>
     <row r="154" spans="1:7">
       <c r="A154" s="11" t="s">
-        <v>393</v>
+        <v>417</v>
       </c>
       <c r="B154" s="12"/>
-      <c r="C154" s="12"/>
+      <c r="C154" s="12" t="s">
+        <v>418</v>
+      </c>
       <c r="D154" s="13" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
       <c r="E154" s="16" t="s">
-        <v>393</v>
+        <v>417</v>
       </c>
       <c r="F154" s="14"/>
       <c r="G154" s="15"/>
     </row>
     <row r="155" spans="1:7">
       <c r="A155" s="11" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="B155" s="12"/>
       <c r="C155" s="12"/>
       <c r="D155" s="13" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
       <c r="E155" s="11" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="F155" s="14"/>
       <c r="G155" s="15"/>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="11" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="B156" s="12"/>
-      <c r="C156" s="12"/>
+      <c r="C156" s="12" t="s">
+        <v>423</v>
+      </c>
       <c r="D156" s="13" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="E156" s="11"/>
       <c r="F156" s="14"/>
@@ -6917,12 +7122,14 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157" s="11" t="s">
-        <v>399</v>
+        <v>425</v>
       </c>
       <c r="B157" s="12"/>
-      <c r="C157" s="12"/>
+      <c r="C157" s="12" t="s">
+        <v>426</v>
+      </c>
       <c r="D157" s="13" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="E157" s="11"/>
       <c r="F157" s="14"/>
@@ -6930,59 +7137,67 @@
     </row>
     <row r="158" s="4" customFormat="1" spans="1:7">
       <c r="A158" s="29" t="s">
-        <v>401</v>
+        <v>428</v>
       </c>
       <c r="B158" s="45"/>
-      <c r="C158" s="45"/>
+      <c r="C158" s="45" t="s">
+        <v>429</v>
+      </c>
       <c r="D158" s="46" t="s">
-        <v>402</v>
+        <v>430</v>
       </c>
       <c r="E158" s="28" t="s">
-        <v>403</v>
+        <v>431</v>
       </c>
       <c r="F158" s="29" t="s">
-        <v>404</v>
+        <v>432</v>
       </c>
       <c r="G158" s="47"/>
     </row>
     <row r="159" s="4" customFormat="1" spans="1:7">
       <c r="A159" s="29" t="s">
-        <v>405</v>
+        <v>433</v>
       </c>
       <c r="B159" s="45"/>
-      <c r="C159" s="45"/>
+      <c r="C159" s="45" t="s">
+        <v>429</v>
+      </c>
       <c r="D159" s="46" t="s">
-        <v>406</v>
+        <v>434</v>
       </c>
       <c r="E159" s="29" t="s">
-        <v>407</v>
+        <v>435</v>
       </c>
       <c r="F159" s="29"/>
       <c r="G159" s="47"/>
     </row>
     <row r="160" s="4" customFormat="1" spans="1:7">
       <c r="A160" s="29" t="s">
-        <v>408</v>
+        <v>436</v>
       </c>
       <c r="B160" s="45"/>
-      <c r="C160" s="45"/>
+      <c r="C160" s="45" t="s">
+        <v>429</v>
+      </c>
       <c r="D160" s="46" t="s">
-        <v>409</v>
+        <v>437</v>
       </c>
       <c r="E160" s="28" t="s">
-        <v>410</v>
+        <v>438</v>
       </c>
       <c r="F160" s="29"/>
       <c r="G160" s="47"/>
     </row>
     <row r="161" spans="1:7">
       <c r="A161" s="11" t="s">
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="B161" s="12"/>
-      <c r="C161" s="12"/>
+      <c r="C161" s="12" t="s">
+        <v>440</v>
+      </c>
       <c r="D161" s="13" t="s">
-        <v>412</v>
+        <v>441</v>
       </c>
       <c r="E161" s="11"/>
       <c r="F161" s="14"/>
@@ -6990,12 +7205,14 @@
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="16" t="s">
-        <v>413</v>
+        <v>442</v>
       </c>
       <c r="B162" s="12"/>
-      <c r="C162" s="12"/>
+      <c r="C162" s="12" t="s">
+        <v>443</v>
+      </c>
       <c r="D162" s="13" t="s">
-        <v>414</v>
+        <v>444</v>
       </c>
       <c r="E162" s="11"/>
       <c r="F162" s="14"/>
@@ -7003,27 +7220,29 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="11" t="s">
-        <v>415</v>
+        <v>445</v>
       </c>
       <c r="B163" s="12"/>
-      <c r="C163" s="12"/>
+      <c r="C163" s="12" t="s">
+        <v>446</v>
+      </c>
       <c r="D163" s="13" t="s">
-        <v>416</v>
+        <v>447</v>
       </c>
       <c r="E163" s="11" t="s">
-        <v>415</v>
+        <v>445</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="15"/>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="11" t="s">
-        <v>417</v>
+        <v>448</v>
       </c>
       <c r="B164" s="12"/>
       <c r="C164" s="12"/>
       <c r="D164" s="13" t="s">
-        <v>418</v>
+        <v>449</v>
       </c>
       <c r="E164" s="11"/>
       <c r="F164" s="14"/>
@@ -7031,12 +7250,12 @@
     </row>
     <row r="165" spans="1:7">
       <c r="A165" s="11" t="s">
-        <v>419</v>
+        <v>450</v>
       </c>
       <c r="B165" s="12"/>
       <c r="C165" s="12"/>
       <c r="D165" s="13" t="s">
-        <v>420</v>
+        <v>451</v>
       </c>
       <c r="E165" s="11"/>
       <c r="F165" s="14"/>
@@ -7044,27 +7263,27 @@
     </row>
     <row r="166" spans="1:7">
       <c r="A166" s="11" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
       <c r="B166" s="12"/>
       <c r="C166" s="12"/>
       <c r="D166" s="13" t="s">
-        <v>422</v>
+        <v>453</v>
       </c>
       <c r="E166" s="11" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
       <c r="F166" s="14"/>
       <c r="G166" s="15"/>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" s="11" t="s">
-        <v>423</v>
+        <v>454</v>
       </c>
       <c r="B167" s="12"/>
       <c r="C167" s="12"/>
       <c r="D167" s="13" t="s">
-        <v>424</v>
+        <v>455</v>
       </c>
       <c r="E167" s="11"/>
       <c r="F167" s="14"/>
@@ -7072,12 +7291,14 @@
     </row>
     <row r="168" spans="1:7">
       <c r="A168" s="16" t="s">
-        <v>425</v>
+        <v>456</v>
       </c>
       <c r="B168" s="12"/>
-      <c r="C168" s="12"/>
+      <c r="C168" s="12" t="s">
+        <v>457</v>
+      </c>
       <c r="D168" s="13" t="s">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c r="E168" s="11"/>
       <c r="F168" s="14"/>
@@ -7085,12 +7306,12 @@
     </row>
     <row r="169" spans="1:7">
       <c r="A169" s="11" t="s">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c r="B169" s="12"/>
       <c r="C169" s="12"/>
       <c r="D169" s="13" t="s">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c r="E169" s="11"/>
       <c r="F169" s="14"/>
@@ -7098,12 +7319,14 @@
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="16" t="s">
-        <v>429</v>
+        <v>461</v>
       </c>
       <c r="B170" s="12"/>
-      <c r="C170" s="12"/>
+      <c r="C170" s="12" t="s">
+        <v>462</v>
+      </c>
       <c r="D170" s="13" t="s">
-        <v>430</v>
+        <v>463</v>
       </c>
       <c r="E170" s="11"/>
       <c r="F170" s="14"/>
@@ -7111,12 +7334,12 @@
     </row>
     <row r="171" spans="1:7">
       <c r="A171" s="11" t="s">
-        <v>431</v>
+        <v>464</v>
       </c>
       <c r="B171" s="12"/>
       <c r="C171" s="12"/>
       <c r="D171" s="13" t="s">
-        <v>432</v>
+        <v>465</v>
       </c>
       <c r="E171" s="11"/>
       <c r="F171" s="14"/>
@@ -7124,12 +7347,12 @@
     </row>
     <row r="172" spans="1:7">
       <c r="A172" s="11" t="s">
-        <v>433</v>
+        <v>466</v>
       </c>
       <c r="B172" s="12"/>
       <c r="C172" s="12"/>
       <c r="D172" s="13" t="s">
-        <v>434</v>
+        <v>467</v>
       </c>
       <c r="E172" s="11"/>
       <c r="F172" s="14"/>
@@ -7137,76 +7360,78 @@
     </row>
     <row r="173" spans="1:7">
       <c r="A173" s="11" t="s">
-        <v>435</v>
+        <v>468</v>
       </c>
       <c r="B173" s="12"/>
       <c r="C173" s="12"/>
       <c r="D173" s="13" t="s">
-        <v>436</v>
+        <v>469</v>
       </c>
       <c r="E173" s="11" t="s">
-        <v>435</v>
+        <v>468</v>
       </c>
       <c r="F173" s="14" t="s">
-        <v>437</v>
+        <v>470</v>
       </c>
       <c r="G173" s="15"/>
     </row>
     <row r="174" spans="1:7">
       <c r="A174" s="11" t="s">
-        <v>438</v>
+        <v>471</v>
       </c>
       <c r="B174" s="12"/>
       <c r="C174" s="12"/>
       <c r="D174" s="13" t="s">
-        <v>439</v>
+        <v>472</v>
       </c>
       <c r="E174" s="11" t="s">
-        <v>438</v>
+        <v>471</v>
       </c>
       <c r="F174" s="14"/>
       <c r="G174" s="15"/>
     </row>
     <row r="175" spans="1:7">
       <c r="A175" s="16" t="s">
-        <v>440</v>
+        <v>473</v>
       </c>
       <c r="B175" s="12"/>
-      <c r="C175" s="12"/>
+      <c r="C175" s="12" t="s">
+        <v>138</v>
+      </c>
       <c r="D175" s="13" t="s">
-        <v>441</v>
+        <v>474</v>
       </c>
       <c r="E175" s="11" t="s">
-        <v>440</v>
+        <v>473</v>
       </c>
       <c r="F175" s="14"/>
       <c r="G175" s="15"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="11" t="s">
-        <v>442</v>
+        <v>475</v>
       </c>
       <c r="B176" s="12"/>
       <c r="C176" s="12"/>
       <c r="D176" s="13" t="s">
-        <v>443</v>
+        <v>476</v>
       </c>
       <c r="E176" s="14" t="s">
-        <v>442</v>
+        <v>475</v>
       </c>
       <c r="F176" s="14" t="s">
-        <v>444</v>
+        <v>477</v>
       </c>
       <c r="G176" s="15"/>
     </row>
     <row r="177" spans="1:7">
       <c r="A177" s="11" t="s">
-        <v>445</v>
+        <v>478</v>
       </c>
       <c r="B177" s="12"/>
       <c r="C177" s="12"/>
       <c r="D177" s="13" t="s">
-        <v>446</v>
+        <v>479</v>
       </c>
       <c r="E177" s="11"/>
       <c r="F177" s="14"/>
@@ -7214,12 +7439,14 @@
     </row>
     <row r="178" spans="1:7">
       <c r="A178" s="11" t="s">
-        <v>447</v>
+        <v>480</v>
       </c>
       <c r="B178" s="12"/>
-      <c r="C178" s="12"/>
+      <c r="C178" s="12" t="s">
+        <v>481</v>
+      </c>
       <c r="D178" s="13" t="s">
-        <v>448</v>
+        <v>482</v>
       </c>
       <c r="E178" s="11"/>
       <c r="F178" s="14"/>
@@ -7227,12 +7454,14 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179" s="16" t="s">
-        <v>449</v>
+        <v>483</v>
       </c>
       <c r="B179" s="12"/>
-      <c r="C179" s="12"/>
+      <c r="C179" s="12" t="s">
+        <v>484</v>
+      </c>
       <c r="D179" s="13" t="s">
-        <v>450</v>
+        <v>485</v>
       </c>
       <c r="E179" s="11"/>
       <c r="F179" s="14"/>
@@ -7240,29 +7469,33 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180" s="11" t="s">
-        <v>451</v>
+        <v>486</v>
       </c>
       <c r="B180" s="12"/>
-      <c r="C180" s="12"/>
+      <c r="C180" s="12" t="s">
+        <v>487</v>
+      </c>
       <c r="D180" s="13" t="s">
-        <v>452</v>
+        <v>488</v>
       </c>
       <c r="E180" s="11" t="s">
-        <v>451</v>
+        <v>486</v>
       </c>
       <c r="F180" s="14" t="s">
-        <v>451</v>
+        <v>486</v>
       </c>
       <c r="G180" s="15"/>
     </row>
     <row r="181" spans="1:7">
       <c r="A181" s="11" t="s">
-        <v>453</v>
+        <v>489</v>
       </c>
       <c r="B181" s="12"/>
-      <c r="C181" s="12"/>
+      <c r="C181" s="12" t="s">
+        <v>487</v>
+      </c>
       <c r="D181" s="13" t="s">
-        <v>454</v>
+        <v>490</v>
       </c>
       <c r="E181" s="11"/>
       <c r="F181" s="14"/>
@@ -7270,57 +7503,59 @@
     </row>
     <row r="182" spans="1:7">
       <c r="A182" s="11" t="s">
-        <v>455</v>
+        <v>491</v>
       </c>
       <c r="B182" s="12"/>
-      <c r="C182" s="12"/>
+      <c r="C182" s="12" t="s">
+        <v>487</v>
+      </c>
       <c r="D182" s="13" t="s">
-        <v>456</v>
+        <v>492</v>
       </c>
       <c r="E182" s="11"/>
       <c r="F182" s="14" t="s">
-        <v>457</v>
+        <v>493</v>
       </c>
       <c r="G182" s="15"/>
     </row>
     <row r="183" spans="1:7">
       <c r="A183" s="11" t="s">
-        <v>458</v>
+        <v>494</v>
       </c>
       <c r="B183" s="12"/>
       <c r="C183" s="12"/>
       <c r="D183" s="13" t="s">
-        <v>459</v>
+        <v>495</v>
       </c>
       <c r="E183" s="11" t="s">
-        <v>458</v>
+        <v>494</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="15"/>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" s="11" t="s">
-        <v>460</v>
+        <v>496</v>
       </c>
       <c r="B184" s="12"/>
       <c r="C184" s="12"/>
       <c r="D184" s="13" t="s">
-        <v>461</v>
+        <v>497</v>
       </c>
       <c r="E184" s="11" t="s">
-        <v>460</v>
+        <v>496</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="15"/>
     </row>
     <row r="185" spans="1:7">
       <c r="A185" s="13" t="s">
-        <v>462</v>
+        <v>498</v>
       </c>
       <c r="B185" s="32"/>
       <c r="C185" s="32"/>
       <c r="D185" s="13" t="s">
-        <v>463</v>
+        <v>499</v>
       </c>
       <c r="E185" s="13"/>
       <c r="F185" s="21"/>
@@ -7328,93 +7563,105 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186" s="11" t="s">
-        <v>464</v>
+        <v>500</v>
       </c>
       <c r="B186" s="12"/>
-      <c r="C186" s="12"/>
+      <c r="C186" s="12" t="s">
+        <v>501</v>
+      </c>
       <c r="D186" s="13" t="s">
-        <v>465</v>
+        <v>502</v>
       </c>
       <c r="E186" s="11" t="s">
-        <v>464</v>
+        <v>500</v>
       </c>
       <c r="F186" s="14"/>
       <c r="G186" s="15"/>
     </row>
     <row r="187" spans="1:7">
       <c r="A187" s="11" t="s">
-        <v>466</v>
+        <v>503</v>
       </c>
       <c r="B187" s="12"/>
-      <c r="C187" s="12"/>
+      <c r="C187" s="12" t="s">
+        <v>504</v>
+      </c>
       <c r="D187" s="13" t="s">
-        <v>467</v>
+        <v>505</v>
       </c>
       <c r="E187" s="16" t="s">
-        <v>468</v>
+        <v>506</v>
       </c>
       <c r="F187" s="14"/>
       <c r="G187" s="15"/>
     </row>
     <row r="188" spans="1:7">
       <c r="A188" s="16" t="s">
-        <v>469</v>
+        <v>507</v>
       </c>
       <c r="B188" s="12"/>
-      <c r="C188" s="12"/>
+      <c r="C188" s="12" t="s">
+        <v>508</v>
+      </c>
       <c r="D188" s="13" t="s">
-        <v>470</v>
+        <v>509</v>
       </c>
       <c r="E188" s="11" t="s">
-        <v>469</v>
+        <v>507</v>
       </c>
       <c r="F188" s="14"/>
       <c r="G188" s="15"/>
     </row>
     <row r="189" s="2" customFormat="1" spans="1:7">
       <c r="A189" s="28" t="s">
-        <v>471</v>
+        <v>510</v>
       </c>
       <c r="B189" s="26"/>
-      <c r="C189" s="26"/>
+      <c r="C189" s="26" t="s">
+        <v>511</v>
+      </c>
       <c r="D189" s="27" t="s">
-        <v>472</v>
+        <v>512</v>
       </c>
       <c r="E189" s="25" t="s">
-        <v>473</v>
+        <v>513</v>
       </c>
       <c r="F189" s="29"/>
       <c r="G189" s="30"/>
     </row>
     <row r="190" s="2" customFormat="1" spans="1:7">
       <c r="A190" s="25" t="s">
-        <v>474</v>
+        <v>514</v>
       </c>
       <c r="B190" s="26"/>
-      <c r="C190" s="26"/>
+      <c r="C190" s="26" t="s">
+        <v>515</v>
+      </c>
       <c r="D190" s="27" t="s">
-        <v>475</v>
+        <v>516</v>
       </c>
       <c r="E190" s="25" t="s">
-        <v>474</v>
+        <v>514</v>
       </c>
       <c r="F190" s="29"/>
       <c r="G190" s="30"/>
     </row>
     <row r="191" s="2" customFormat="1" spans="1:7">
       <c r="A191" s="25" t="s">
-        <v>476</v>
+        <v>517</v>
       </c>
       <c r="B191" s="26"/>
-      <c r="C191" s="26"/>
+      <c r="C191" s="26" t="s">
+        <v>515</v>
+      </c>
       <c r="D191" s="27" t="s">
-        <v>477</v>
+        <v>518</v>
       </c>
       <c r="E191" s="25" t="s">
-        <v>476</v>
+        <v>517</v>
       </c>
       <c r="F191" s="29" t="s">
-        <v>476</v>
+        <v>517</v>
       </c>
       <c r="G191" s="30"/>
     </row>
@@ -7426,19 +7673,19 @@
       <c r="C192" s="26"/>
       <c r="D192" s="27"/>
       <c r="E192" s="25" t="s">
-        <v>478</v>
+        <v>519</v>
       </c>
       <c r="F192" s="29"/>
       <c r="G192" s="30"/>
     </row>
     <row r="193" s="2" customFormat="1" spans="1:7">
       <c r="A193" s="25" t="s">
-        <v>479</v>
+        <v>520</v>
       </c>
       <c r="B193" s="26"/>
       <c r="C193" s="26"/>
       <c r="D193" s="27" t="s">
-        <v>480</v>
+        <v>521</v>
       </c>
       <c r="E193" s="25"/>
       <c r="F193" s="29"/>
@@ -7446,44 +7693,48 @@
     </row>
     <row r="194" s="2" customFormat="1" spans="1:7">
       <c r="A194" s="25" t="s">
-        <v>481</v>
+        <v>522</v>
       </c>
       <c r="B194" s="26"/>
       <c r="C194" s="26"/>
       <c r="D194" s="27" t="s">
-        <v>482</v>
+        <v>523</v>
       </c>
       <c r="E194" s="25" t="s">
-        <v>481</v>
+        <v>522</v>
       </c>
       <c r="F194" s="29"/>
       <c r="G194" s="30"/>
     </row>
     <row r="195" s="2" customFormat="1" spans="1:7">
       <c r="A195" s="28" t="s">
-        <v>483</v>
+        <v>524</v>
       </c>
       <c r="B195" s="26"/>
-      <c r="C195" s="26"/>
+      <c r="C195" s="26" t="s">
+        <v>525</v>
+      </c>
       <c r="D195" s="27" t="s">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="E195" s="25" t="s">
-        <v>483</v>
+        <v>524</v>
       </c>
       <c r="F195" s="29" t="s">
-        <v>483</v>
+        <v>524</v>
       </c>
       <c r="G195" s="30"/>
     </row>
     <row r="196" s="2" customFormat="1" spans="1:7">
       <c r="A196" s="28" t="s">
-        <v>485</v>
+        <v>527</v>
       </c>
       <c r="B196" s="26"/>
-      <c r="C196" s="26"/>
+      <c r="C196" s="26" t="s">
+        <v>528</v>
+      </c>
       <c r="D196" s="27" t="s">
-        <v>486</v>
+        <v>529</v>
       </c>
       <c r="E196" s="25"/>
       <c r="F196" s="29"/>
@@ -7491,27 +7742,29 @@
     </row>
     <row r="197" s="2" customFormat="1" spans="1:7">
       <c r="A197" s="28" t="s">
-        <v>487</v>
+        <v>530</v>
       </c>
       <c r="B197" s="26"/>
-      <c r="C197" s="26"/>
+      <c r="C197" s="26" t="s">
+        <v>531</v>
+      </c>
       <c r="D197" s="27" t="s">
-        <v>488</v>
+        <v>532</v>
       </c>
       <c r="E197" s="28" t="s">
-        <v>489</v>
+        <v>533</v>
       </c>
       <c r="F197" s="29"/>
       <c r="G197" s="30"/>
     </row>
     <row r="198" s="2" customFormat="1" spans="1:7">
       <c r="A198" s="25" t="s">
-        <v>490</v>
+        <v>534</v>
       </c>
       <c r="B198" s="26"/>
       <c r="C198" s="26"/>
       <c r="D198" s="27" t="s">
-        <v>491</v>
+        <v>535</v>
       </c>
       <c r="E198" s="25"/>
       <c r="F198" s="29"/>
@@ -7525,19 +7778,21 @@
       <c r="C199" s="26"/>
       <c r="D199" s="27"/>
       <c r="E199" s="25" t="s">
-        <v>492</v>
+        <v>536</v>
       </c>
       <c r="F199" s="29"/>
       <c r="G199" s="30"/>
     </row>
     <row r="200" s="2" customFormat="1" spans="1:7">
       <c r="A200" s="28" t="s">
-        <v>493</v>
+        <v>537</v>
       </c>
       <c r="B200" s="26"/>
-      <c r="C200" s="26"/>
+      <c r="C200" s="26" t="s">
+        <v>538</v>
+      </c>
       <c r="D200" s="27" t="s">
-        <v>494</v>
+        <v>539</v>
       </c>
       <c r="E200" s="25"/>
       <c r="F200" s="29"/>
@@ -7545,15 +7800,15 @@
     </row>
     <row r="201" s="2" customFormat="1" spans="1:7">
       <c r="A201" s="28" t="s">
-        <v>495</v>
+        <v>540</v>
       </c>
       <c r="B201" s="26"/>
       <c r="C201" s="26"/>
       <c r="D201" s="27" t="s">
-        <v>496</v>
+        <v>541</v>
       </c>
       <c r="E201" s="28" t="s">
-        <v>497</v>
+        <v>542</v>
       </c>
       <c r="F201" s="29"/>
       <c r="G201" s="30"/>
@@ -7566,19 +7821,19 @@
       <c r="C202" s="26"/>
       <c r="D202" s="27"/>
       <c r="E202" s="16" t="s">
-        <v>498</v>
+        <v>543</v>
       </c>
       <c r="F202" s="29"/>
       <c r="G202" s="30"/>
     </row>
     <row r="203" s="2" customFormat="1" spans="1:7">
       <c r="A203" s="25" t="s">
-        <v>499</v>
+        <v>544</v>
       </c>
       <c r="B203" s="26"/>
       <c r="C203" s="26"/>
       <c r="D203" s="27" t="s">
-        <v>500</v>
+        <v>545</v>
       </c>
       <c r="E203" s="25"/>
       <c r="F203" s="29"/>
@@ -7586,7 +7841,7 @@
     </row>
     <row r="204" spans="1:7">
       <c r="A204" s="25" t="s">
-        <v>501</v>
+        <v>546</v>
       </c>
       <c r="B204" s="26"/>
       <c r="C204" s="26"/>
@@ -7603,64 +7858,66 @@
       <c r="C205" s="26"/>
       <c r="D205" s="27"/>
       <c r="E205" s="25" t="s">
-        <v>502</v>
+        <v>547</v>
       </c>
       <c r="F205" s="14"/>
       <c r="G205" s="30"/>
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="11" t="s">
-        <v>503</v>
+        <v>548</v>
       </c>
       <c r="B206" s="12"/>
       <c r="C206" s="12"/>
       <c r="D206" s="13" t="s">
-        <v>504</v>
+        <v>549</v>
       </c>
       <c r="E206" s="11" t="s">
-        <v>505</v>
+        <v>550</v>
       </c>
       <c r="F206" s="14"/>
       <c r="G206" s="15"/>
     </row>
     <row r="207" spans="1:7">
       <c r="A207" s="11" t="s">
-        <v>506</v>
+        <v>551</v>
       </c>
       <c r="B207" s="12"/>
       <c r="C207" s="12"/>
       <c r="D207" s="13" t="s">
-        <v>507</v>
+        <v>552</v>
       </c>
       <c r="E207" s="16" t="s">
-        <v>506</v>
+        <v>551</v>
       </c>
       <c r="F207" s="14"/>
       <c r="G207" s="15"/>
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="11" t="s">
-        <v>508</v>
+        <v>553</v>
       </c>
       <c r="B208" s="12"/>
       <c r="C208" s="12"/>
       <c r="D208" s="13" t="s">
-        <v>509</v>
+        <v>554</v>
       </c>
       <c r="E208" s="16" t="s">
-        <v>510</v>
+        <v>555</v>
       </c>
       <c r="F208" s="14"/>
       <c r="G208" s="15"/>
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="16" t="s">
-        <v>511</v>
+        <v>556</v>
       </c>
       <c r="B209" s="12"/>
-      <c r="C209" s="12"/>
+      <c r="C209" s="12" t="s">
+        <v>557</v>
+      </c>
       <c r="D209" s="13" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="E209" s="11"/>
       <c r="F209" s="14"/>
@@ -7668,74 +7925,74 @@
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="11" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
       <c r="B210" s="12"/>
       <c r="C210" s="12"/>
       <c r="D210" s="13" t="s">
-        <v>513</v>
+        <v>559</v>
       </c>
       <c r="E210" s="11" t="s">
-        <v>512</v>
+        <v>558</v>
       </c>
       <c r="F210" s="14" t="s">
-        <v>514</v>
+        <v>560</v>
       </c>
       <c r="G210" s="15"/>
     </row>
     <row r="211" spans="1:7">
       <c r="A211" s="11" t="s">
-        <v>515</v>
+        <v>561</v>
       </c>
       <c r="B211" s="12"/>
       <c r="C211" s="12"/>
       <c r="D211" s="13" t="s">
-        <v>516</v>
+        <v>562</v>
       </c>
       <c r="E211" s="11" t="s">
-        <v>515</v>
+        <v>561</v>
       </c>
       <c r="F211" s="14"/>
       <c r="G211" s="15"/>
     </row>
     <row r="212" spans="1:7">
       <c r="A212" s="11" t="s">
-        <v>517</v>
+        <v>563</v>
       </c>
       <c r="B212" s="12"/>
       <c r="C212" s="12"/>
       <c r="D212" s="13" t="s">
-        <v>518</v>
+        <v>564</v>
       </c>
       <c r="E212" s="11" t="s">
-        <v>517</v>
+        <v>563</v>
       </c>
       <c r="F212" s="14"/>
       <c r="G212" s="15"/>
     </row>
     <row r="213" spans="1:7">
       <c r="A213" s="11" t="s">
-        <v>519</v>
+        <v>565</v>
       </c>
       <c r="B213" s="12"/>
       <c r="C213" s="12"/>
       <c r="D213" s="13" t="s">
-        <v>520</v>
+        <v>566</v>
       </c>
       <c r="E213" s="11" t="s">
-        <v>519</v>
+        <v>565</v>
       </c>
       <c r="F213" s="14"/>
       <c r="G213" s="15"/>
     </row>
     <row r="214" spans="1:7">
       <c r="A214" s="11" t="s">
-        <v>521</v>
+        <v>567</v>
       </c>
       <c r="B214" s="12"/>
       <c r="C214" s="12"/>
       <c r="D214" s="13" t="s">
-        <v>522</v>
+        <v>568</v>
       </c>
       <c r="E214" s="11"/>
       <c r="F214" s="14"/>
@@ -7743,12 +8000,12 @@
     </row>
     <row r="215" spans="1:7">
       <c r="A215" s="11" t="s">
-        <v>523</v>
+        <v>569</v>
       </c>
       <c r="B215" s="12"/>
       <c r="C215" s="12"/>
       <c r="D215" s="13" t="s">
-        <v>524</v>
+        <v>570</v>
       </c>
       <c r="E215" s="11"/>
       <c r="F215" s="14"/>
@@ -7762,7 +8019,7 @@
       <c r="C216" s="12"/>
       <c r="D216" s="13"/>
       <c r="E216" s="11" t="s">
-        <v>525</v>
+        <v>571</v>
       </c>
       <c r="F216" s="14"/>
       <c r="G216" s="15"/>
@@ -7775,19 +8032,19 @@
       <c r="C217" s="12"/>
       <c r="D217" s="13"/>
       <c r="E217" s="11" t="s">
-        <v>526</v>
+        <v>572</v>
       </c>
       <c r="F217" s="14"/>
       <c r="G217" s="15"/>
     </row>
     <row r="218" spans="1:7">
       <c r="A218" s="11" t="s">
-        <v>527</v>
+        <v>573</v>
       </c>
       <c r="B218" s="12"/>
       <c r="C218" s="12"/>
       <c r="D218" s="13" t="s">
-        <v>528</v>
+        <v>574</v>
       </c>
       <c r="E218" s="11"/>
       <c r="F218" s="14"/>
@@ -7795,33 +8052,33 @@
     </row>
     <row r="219" spans="1:7">
       <c r="A219" s="11" t="s">
-        <v>529</v>
+        <v>575</v>
       </c>
       <c r="B219" s="12"/>
       <c r="C219" s="12"/>
       <c r="D219" s="13" t="s">
-        <v>530</v>
+        <v>576</v>
       </c>
       <c r="E219" s="11" t="s">
-        <v>529</v>
+        <v>575</v>
       </c>
       <c r="F219" s="14"/>
       <c r="G219" s="15"/>
     </row>
     <row r="220" s="2" customFormat="1" spans="1:7">
       <c r="A220" s="27" t="s">
-        <v>531</v>
+        <v>577</v>
       </c>
       <c r="B220" s="48"/>
       <c r="C220" s="48"/>
       <c r="D220" s="27" t="s">
-        <v>532</v>
+        <v>578</v>
       </c>
       <c r="E220" s="27" t="s">
-        <v>533</v>
+        <v>579</v>
       </c>
       <c r="F220" s="46" t="s">
-        <v>533</v>
+        <v>579</v>
       </c>
       <c r="G220" s="27"/>
     </row>
@@ -7833,19 +8090,19 @@
       <c r="C221" s="48"/>
       <c r="D221" s="27"/>
       <c r="E221" s="49" t="s">
-        <v>534</v>
+        <v>580</v>
       </c>
       <c r="F221" s="46"/>
       <c r="G221" s="27"/>
     </row>
     <row r="222" spans="1:7">
       <c r="A222" s="11" t="s">
-        <v>535</v>
+        <v>581</v>
       </c>
       <c r="B222" s="12"/>
       <c r="C222" s="12"/>
       <c r="D222" s="13" t="s">
-        <v>536</v>
+        <v>582</v>
       </c>
       <c r="E222" s="11"/>
       <c r="F222" s="14"/>
@@ -7853,12 +8110,14 @@
     </row>
     <row r="223" spans="1:7">
       <c r="A223" s="16" t="s">
-        <v>537</v>
+        <v>583</v>
       </c>
       <c r="B223" s="12"/>
-      <c r="C223" s="12"/>
+      <c r="C223" s="12" t="s">
+        <v>584</v>
+      </c>
       <c r="D223" s="13" t="s">
-        <v>538</v>
+        <v>585</v>
       </c>
       <c r="E223" s="11"/>
       <c r="F223" s="14"/>

</xml_diff>